<commit_message>
perubahan sedikit (test commit, gus)
</commit_message>
<xml_diff>
--- a/rpt/Inventory Report with  Sub-Category.xlsx
+++ b/rpt/Inventory Report with  Sub-Category.xlsx
@@ -26,7 +26,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -434,10 +434,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7:G7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,141 +452,149 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>5</v>
-      </c>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
+      <c r="B4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>12855.53</v>
-      </c>
-      <c r="G4" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>50000</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>12855.53</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="8" t="n">
-        <v>50</v>
-      </c>
-      <c r="F8" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="G8" s="9" t="n">
-        <v>1500</v>
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.445138888888889" right="0.296527777777778" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -607,7 +615,7 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C7:G7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
adding more test. trial clone
</commit_message>
<xml_diff>
--- a/rpt/Inventory Report with  Sub-Category.xlsx
+++ b/rpt/Inventory Report with  Sub-Category.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,7 +615,7 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fxlpalmtree.py copied from s.i.o.d without FXL.core
</commit_message>
<xml_diff>
--- a/rpt/Inventory Report with  Sub-Category.xlsx
+++ b/rpt/Inventory Report with  Sub-Category.xlsx
@@ -26,7 +26,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0">
+    <comment ref="C11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,11 +135,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t xml:space="preserve">Inventory Report Category with Sub-Category</t>
   </si>
   <si>
+    <t xml:space="preserve">Sub-judul, merged-cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">~Item</t>
   </si>
   <si>
@@ -129,12 +158,6 @@
     <t xml:space="preserve">MENU PAKET</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity         :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 PAX</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cost Value  :</t>
   </si>
   <si>
@@ -159,34 +182,49 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Recipe Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jadi brp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~Item.BoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SY0029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NANGKA SAYUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~Item.BoM:F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Report Category with Sub-Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category        :</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantity Rcp</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SY0029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NANGKA SAYUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Report Category with Sub-Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category        :</t>
-  </si>
-  <si>
     <t xml:space="preserve">Qty Sales</t>
   </si>
   <si>
     <t xml:space="preserve">Total Rcp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAX</t>
   </si>
   <si>
     <t xml:space="preserve">gram</t>
@@ -271,12 +309,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$Rp-421]#,##0.00;[RED]\([$Rp-421]#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="[$-421]GE\nER&quot;al&quot;"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="[$-421]GE\nER&quot;al&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -311,6 +350,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -326,12 +371,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -360,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,39 +425,51 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,10 +498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,9 +510,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="2.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="2.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,7 +526,9 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -467,134 +538,172 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>12855.53</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>50000</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>12855.53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>50000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="8" t="n">
-        <v>50</v>
-      </c>
-      <c r="F9" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>1500</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <f aca="false">F11/E11</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10" t="n">
+        <f aca="false">MIN(G11:G11)</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:F2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.445138888888889" right="0.296527777777778" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -614,25 +723,27 @@
   </sheetPr>
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -644,335 +755,335 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="8" t="n">
-        <v>50</v>
-      </c>
-      <c r="F8" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>2500</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="F9" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>25</v>
+      <c r="F9" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>600</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="8" t="n">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="F10" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>25</v>
+      <c r="F10" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>500</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="n">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="n">
         <v>0.2</v>
       </c>
-      <c r="F11" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>25</v>
+      <c r="F11" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="8" t="n">
+        <v>39</v>
+      </c>
+      <c r="E12" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F12" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>25</v>
+      <c r="F12" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>250</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="8" t="n">
+        <v>41</v>
+      </c>
+      <c r="E13" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="F13" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>25</v>
+      <c r="F13" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1250</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="8" t="n">
+        <v>43</v>
+      </c>
+      <c r="E14" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>25</v>
+      <c r="F14" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>250</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="8" t="n">
+        <v>45</v>
+      </c>
+      <c r="E15" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="F15" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>25</v>
+      <c r="F15" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="8" t="n">
+        <v>48</v>
+      </c>
+      <c r="E16" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="F16" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>25</v>
+      <c r="F16" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>25</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="8" t="n">
+        <v>51</v>
+      </c>
+      <c r="E17" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>25</v>
+      <c r="F17" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>750</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="8" t="n">
+        <v>53</v>
+      </c>
+      <c r="E18" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>25</v>
+      <c r="F18" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>150</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="8" t="n">
+        <v>55</v>
+      </c>
+      <c r="E19" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F19" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>25</v>
+      <c r="F19" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>250</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="E20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
palmtree is ready for next level.
</commit_message>
<xml_diff>
--- a/rpt/Inventory Report with  Sub-Category.xlsx
+++ b/rpt/Inventory Report with  Sub-Category.xlsx
@@ -500,8 +500,8 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>